<commit_message>
Métricas e Testes das mesmas - FEITO
</commit_message>
<xml_diff>
--- a/CodeQualityAssessor/ficheiro_excel.xlsx
+++ b/CodeQualityAssessor/ficheiro_excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>MethodID</t>
   </si>
@@ -53,13 +53,10 @@
     <t>App</t>
   </si>
   <si>
-    <t>App()</t>
+    <t>main(String[] args)</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>main(String[] args)</t>
   </si>
   <si>
     <t>memoryRecall()</t>
@@ -116,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -171,22 +168,22 @@
         <v>13</v>
       </c>
       <c r="E2" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="F2" t="n">
-        <v>34.0</v>
+        <v>1.0</v>
       </c>
       <c r="G2" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
       </c>
       <c r="I2" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
@@ -206,22 +203,22 @@
         <v>15</v>
       </c>
       <c r="E3" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="F3" t="n">
-        <v>34.0</v>
+        <v>1.0</v>
       </c>
       <c r="G3" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
       <c r="I3" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
@@ -241,13 +238,13 @@
         <v>16</v>
       </c>
       <c r="E4" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="F4" t="n">
-        <v>34.0</v>
+        <v>1.0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
@@ -259,41 +256,6 @@
         <v>1.0</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>